<commit_message>
fix: new run if invalid input
</commit_message>
<xml_diff>
--- a/src/main/resources/Ergebnisse.xlsx
+++ b/src/main/resources/Ergebnisse.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Blumenroth\ideaProjects\Masterarbeit\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A959F0DA-D1A6-4138-A389-DC8415AF18DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14AA601F-4EC4-4C95-B7D9-8CBE615EBAEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,18 +25,51 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
-  <si>
-    <t>3 DMs</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Alt</t>
   </si>
   <si>
-    <t>Crit</t>
+    <t>3 x 5 x 3 = 7.1594</t>
   </si>
   <si>
-    <t>Average</t>
+    <t>3 x 5 x 6 = 15.6579</t>
+  </si>
+  <si>
+    <t>3 x 10 x 3 = 10.0943</t>
+  </si>
+  <si>
+    <t>3 x 10 x 6 = 22.0693</t>
+  </si>
+  <si>
+    <t>3 x 15 x 3 = 12.0801</t>
+  </si>
+  <si>
+    <t>3 x 15 x 6 = 26.5727</t>
+  </si>
+  <si>
+    <t>6 x 5 x 3 = 10.2501</t>
+  </si>
+  <si>
+    <t>6 x 5 x 6 = 20.5599</t>
+  </si>
+  <si>
+    <t>6 x 10 x 3 = 15.7006</t>
+  </si>
+  <si>
+    <t>6 x 10 x 6 = 30.6834</t>
+  </si>
+  <si>
+    <t>6 x 15 x 3 = 19.9882</t>
+  </si>
+  <si>
+    <t>6 x 15 x 6 = 39.4791</t>
+  </si>
+  <si>
+    <t>DM=3</t>
+  </si>
+  <si>
+    <t>DM=6</t>
   </si>
 </sst>
 </file>
@@ -46,13 +79,19 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -75,9 +114,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -130,7 +172,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="de-DE"/>
-              <a:t>Fuzzy-SAW</a:t>
+              <a:t>Fuzzy-SAW DM=3</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -215,7 +257,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle1!$G$8</c:f>
+              <c:f>Tabelle1!$H$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -232,61 +274,54 @@
               <a:noFill/>
             </a:ln>
             <a:effectLst/>
-            <a:scene3d>
-              <a:camera prst="orthographicFront"/>
-              <a:lightRig rig="threePt" dir="t"/>
-            </a:scene3d>
-            <a:sp3d prstMaterial="matte">
-              <a:bevelT w="0" h="19050"/>
-              <a:bevelB w="0" h="6350"/>
-            </a:sp3d>
+            <a:sp3d/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:numRef>
-              <c:f>Tabelle1!$H$7:$K$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+            <c:multiLvlStrRef>
+              <c:f>Tabelle1!$F$6:$G$8</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="3"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>5</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>10</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>15</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Alt</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$H$8:$K$8</c:f>
+              <c:f>Tabelle1!$H$6:$H$8</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>5.2462</c:v>
+                  <c:v>7.1593999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.3609</c:v>
+                  <c:v>10.0943</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.1593999999999998</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>7.9439000000000002</c:v>
+                  <c:v>12.0801</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-D814-4C29-B1AF-F6CC3F98DA76}"/>
+              <c16:uniqueId val="{00000000-FCF2-4296-8034-FE4D8B835B6C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -295,11 +330,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle1!$G$9</c:f>
+              <c:f>Tabelle1!$I$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -316,202 +351,50 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:numRef>
-              <c:f>Tabelle1!$H$7:$K$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+            <c:multiLvlStrRef>
+              <c:f>Tabelle1!$F$6:$G$8</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="3"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>5</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>10</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>15</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Alt</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$H$9:$K$9</c:f>
+              <c:f>Tabelle1!$I$6:$I$8</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>7.3918999999999997</c:v>
+                  <c:v>15.6579</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.8727999999999998</c:v>
+                  <c:v>22.069299999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.040900000000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>11.0236</c:v>
+                  <c:v>26.572700000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-D814-4C29-B1AF-F6CC3F98DA76}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Tabelle1!$G$10</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>5</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-            <a:sp3d/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:numRef>
-              <c:f>Tabelle1!$H$7:$K$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Tabelle1!$H$10:$K$10</c:f>
-              <c:numCache>
-                <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>9.4822000000000006</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>11.323</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>12.8673</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>14.160299999999999</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-D814-4C29-B1AF-F6CC3F98DA76}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Tabelle1!$G$11</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>6</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent4"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-            <a:scene3d>
-              <a:camera prst="orthographicFront"/>
-              <a:lightRig rig="threePt" dir="t"/>
-            </a:scene3d>
-            <a:sp3d>
-              <a:bevelT w="0" h="0"/>
-            </a:sp3d>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:numRef>
-              <c:f>Tabelle1!$H$7:$K$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Tabelle1!$H$11:$K$11</c:f>
-              <c:numCache>
-                <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>11.509399999999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>13.9377</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>15.6579</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>17.3032</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-D814-4C29-B1AF-F6CC3F98DA76}"/>
+              <c16:uniqueId val="{00000001-FCF2-4296-8034-FE4D8B835B6C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -526,72 +409,17 @@
         <c:gapWidth val="0"/>
         <c:gapDepth val="0"/>
         <c:shape val="box"/>
-        <c:axId val="440329600"/>
-        <c:axId val="440330680"/>
-        <c:axId val="561617768"/>
+        <c:axId val="418125576"/>
+        <c:axId val="418127376"/>
+        <c:axId val="562289488"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="440329600"/>
+        <c:axId val="418125576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="de-DE"/>
-                  <a:t>Alternativen</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -623,7 +451,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="440330680"/>
+        <c:crossAx val="418127376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -631,7 +459,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="440330680"/>
+        <c:axId val="418127376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -651,68 +479,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="de-DE"/>
-                  <a:t>Pfadlängen</a:t>
-                </a:r>
-              </a:p>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:endParaRPr lang="de-DE"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -743,72 +510,17 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="440329600"/>
+        <c:crossAx val="418125576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="561617768"/>
+        <c:axId val="562289488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="de-DE"/>
-                  <a:t>Kriterien</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -839,7 +551,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="440330680"/>
+        <c:crossAx val="418127376"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
       <c:spPr>
@@ -847,11 +559,40 @@
         <a:ln>
           <a:noFill/>
         </a:ln>
-        <a:effectLst>
-          <a:softEdge rad="0"/>
-        </a:effectLst>
+        <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -876,9 +617,507 @@
       </a:solidFill>
       <a:round/>
     </a:ln>
-    <a:effectLst>
-      <a:softEdge rad="1270000"/>
-    </a:effectLst>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE"/>
+              <a:t>Fuzzy-SAW DM=6</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="15"/>
+      <c:rotY val="20"/>
+      <c:depthPercent val="100"/>
+      <c:rAngAx val="1"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:bar3DChart>
+        <c:barDir val="col"/>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$H$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Tabelle1!$F$6:$G$8</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="3"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>5</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>10</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>15</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Alt</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$H$6:$H$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>7.1593999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.0943</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12.0801</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0761-49D4-979B-E6C379006D02}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$I$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Tabelle1!$F$6:$G$8</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="3"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>5</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>10</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>15</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Alt</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$I$6:$I$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>15.6579</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22.069299999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>26.572700000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0761-49D4-979B-E6C379006D02}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="0"/>
+        <c:gapDepth val="0"/>
+        <c:shape val="box"/>
+        <c:axId val="418125576"/>
+        <c:axId val="418127376"/>
+        <c:axId val="562289488"/>
+      </c:bar3DChart>
+      <c:catAx>
+        <c:axId val="418125576"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="418127376"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="418127376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="418125576"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:serAx>
+        <c:axId val="562289488"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="418127376"/>
+        <c:crosses val="autoZero"/>
+      </c:serAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
   </c:spPr>
   <c:txPr>
     <a:bodyPr/>
@@ -938,7 +1177,541 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="286">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="286">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1437,22 +2210,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>539750</xdr:colOff>
+      <xdr:colOff>279400</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>15874</xdr:rowOff>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>206375</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>158749</xdr:rowOff>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Diagramm 4">
+        <xdr:cNvPr id="6" name="Diagramm 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F584028A-FAB0-E071-4D02-3AD87DC17290}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B1AA2A3-82EB-5826-4D47-709D037CE0C9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1465,6 +2238,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Diagramm 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{57A0F56B-837A-4657-997C-0E72D5424383}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1736,321 +2547,160 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L21"/>
+  <dimension ref="A5:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="T3" sqref="T3"/>
+    <sheetView tabSelected="1" topLeftCell="H18" workbookViewId="0">
+      <selection activeCell="S21" sqref="S21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
     <col min="4" max="4" width="8.7265625" style="1"/>
+    <col min="8" max="9" width="11.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="5" spans="1:9">
+      <c r="A5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+      <c r="I5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="G6">
+        <v>5</v>
+      </c>
+      <c r="H6" s="1">
+        <v>7.1593999999999998</v>
+      </c>
+      <c r="I6" s="1">
+        <v>15.6579</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="G7">
+        <v>10</v>
+      </c>
+      <c r="H7" s="1">
+        <v>10.0943</v>
+      </c>
+      <c r="I7" s="1">
+        <v>22.069299999999998</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B2">
+    <row r="8" spans="1:9">
+      <c r="A8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G8">
+        <v>15</v>
+      </c>
+      <c r="H8" s="1">
+        <v>12.0801</v>
+      </c>
+      <c r="I8" s="1">
+        <v>26.572700000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="D25" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H25">
         <v>3</v>
       </c>
-      <c r="C2">
-        <v>3</v>
-      </c>
-      <c r="D2" s="1">
-        <v>5.2462</v>
+      <c r="I25">
+        <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B3">
-        <v>3</v>
-      </c>
-      <c r="C3">
-        <v>4</v>
-      </c>
-      <c r="D3" s="1">
-        <v>7.3918999999999997</v>
+    <row r="26" spans="1:9">
+      <c r="F26" t="s">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>5</v>
+      </c>
+      <c r="H26" s="1">
+        <v>10.2501</v>
+      </c>
+      <c r="I26" s="1">
+        <v>20.559899999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <v>5</v>
-      </c>
-      <c r="D4" s="1">
-        <v>9.4822000000000006</v>
+    <row r="27" spans="1:9">
+      <c r="G27">
+        <v>10</v>
+      </c>
+      <c r="H27" s="1">
+        <v>15.7006</v>
+      </c>
+      <c r="I27" s="1">
+        <v>30.683399999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B5">
-        <v>3</v>
-      </c>
-      <c r="C5">
-        <v>6</v>
-      </c>
-      <c r="D5" s="1">
-        <v>11.509399999999999</v>
+    <row r="28" spans="1:9">
+      <c r="A28" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G28">
+        <v>15</v>
+      </c>
+      <c r="H28" s="1">
+        <v>19.988199999999999</v>
+      </c>
+      <c r="I28" s="1">
+        <v>39.479100000000003</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B6">
-        <v>4</v>
-      </c>
-      <c r="C6">
-        <v>3</v>
-      </c>
-      <c r="D6" s="1">
-        <v>6.3609</v>
+    <row r="29" spans="1:9">
+      <c r="A29" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B7">
-        <v>4</v>
-      </c>
-      <c r="C7">
-        <v>4</v>
-      </c>
-      <c r="D7" s="1">
-        <v>8.8727999999999998</v>
-      </c>
-      <c r="F7" t="s">
-        <v>1</v>
-      </c>
-      <c r="H7">
-        <v>3</v>
-      </c>
-      <c r="I7">
-        <v>4</v>
-      </c>
-      <c r="J7">
-        <v>5</v>
-      </c>
-      <c r="K7">
-        <v>6</v>
-      </c>
-      <c r="L7" t="s">
-        <v>2</v>
+    <row r="30" spans="1:9">
+      <c r="A30" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B8">
-        <v>4</v>
-      </c>
-      <c r="C8">
-        <v>5</v>
-      </c>
-      <c r="D8" s="1">
-        <v>11.323</v>
-      </c>
-      <c r="G8">
-        <v>3</v>
-      </c>
-      <c r="H8" s="1">
-        <v>5.2462</v>
-      </c>
-      <c r="I8" s="1">
-        <v>6.3609</v>
-      </c>
-      <c r="J8" s="1">
-        <v>7.1593999999999998</v>
-      </c>
-      <c r="K8" s="1">
-        <v>7.9439000000000002</v>
+    <row r="31" spans="1:9">
+      <c r="A31" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B9">
-        <v>4</v>
-      </c>
-      <c r="C9">
-        <v>6</v>
-      </c>
-      <c r="D9" s="1">
-        <v>13.9377</v>
-      </c>
-      <c r="G9">
-        <v>4</v>
-      </c>
-      <c r="H9" s="1">
-        <v>7.3918999999999997</v>
-      </c>
-      <c r="I9" s="1">
-        <v>8.8727999999999998</v>
-      </c>
-      <c r="J9" s="1">
-        <v>10.040900000000001</v>
-      </c>
-      <c r="K9" s="1">
-        <v>11.0236</v>
+    <row r="32" spans="1:9">
+      <c r="A32" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B10">
-        <v>5</v>
-      </c>
-      <c r="C10">
-        <v>3</v>
-      </c>
-      <c r="D10" s="1">
-        <v>7.1593999999999998</v>
-      </c>
-      <c r="G10">
-        <v>5</v>
-      </c>
-      <c r="H10" s="1">
-        <v>9.4822000000000006</v>
-      </c>
-      <c r="I10" s="1">
-        <v>11.323</v>
-      </c>
-      <c r="J10" s="1">
-        <v>12.8673</v>
-      </c>
-      <c r="K10" s="1">
-        <v>14.160299999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B11">
-        <v>5</v>
-      </c>
-      <c r="C11">
-        <v>4</v>
-      </c>
-      <c r="D11" s="1">
-        <v>10.040900000000001</v>
-      </c>
-      <c r="G11">
-        <v>6</v>
-      </c>
-      <c r="H11" s="1">
-        <v>11.509399999999999</v>
-      </c>
-      <c r="I11" s="1">
-        <v>13.9377</v>
-      </c>
-      <c r="J11" s="1">
-        <v>15.6579</v>
-      </c>
-      <c r="K11" s="1">
-        <v>17.3032</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B12">
-        <v>5</v>
-      </c>
-      <c r="C12">
-        <v>5</v>
-      </c>
-      <c r="D12" s="1">
-        <v>12.8673</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B13">
-        <v>5</v>
-      </c>
-      <c r="C13">
-        <v>6</v>
-      </c>
-      <c r="D13" s="1">
-        <v>15.6579</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B14">
-        <v>6</v>
-      </c>
-      <c r="C14">
-        <v>3</v>
-      </c>
-      <c r="D14" s="1">
-        <v>7.9439000000000002</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B15">
-        <v>6</v>
-      </c>
-      <c r="C15">
-        <v>4</v>
-      </c>
-      <c r="D15" s="1">
-        <v>11.0236</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B16">
-        <v>6</v>
-      </c>
-      <c r="C16">
-        <v>5</v>
-      </c>
-      <c r="D16" s="1">
-        <v>14.160299999999999</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B17">
-        <v>6</v>
-      </c>
-      <c r="C17">
-        <v>6</v>
-      </c>
-      <c r="D17" s="1">
-        <v>17.3032</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B18">
-        <v>7</v>
-      </c>
-      <c r="C18">
-        <v>3</v>
-      </c>
-      <c r="D18" s="1">
-        <v>8.5389999999999997</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B19">
-        <v>7</v>
-      </c>
-      <c r="C19">
-        <v>4</v>
-      </c>
-      <c r="D19" s="1">
-        <v>11.9466</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B20">
-        <v>7</v>
-      </c>
-      <c r="C20">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B21">
-        <v>7</v>
-      </c>
-      <c r="C21">
-        <v>6</v>
+    <row r="33" spans="1:1">
+      <c r="A33" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>